<commit_message>
Added 5-58, statement of reconciliation. Now doing 5-59...
</commit_message>
<xml_diff>
--- a/Chapter 5/5-60.xlsx
+++ b/Chapter 5/5-60.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\Introduction to Financial Accounting\Chapter 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42C01A9-A14F-4B3F-95EA-E972D4D1BFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AEAEE1-70B9-40EC-9694-62EE36369374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{09ABC647-56DF-4000-8D11-E4AB44AF51F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{09ABC647-56DF-4000-8D11-E4AB44AF51F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Statement of Cash Flow" sheetId="1" r:id="rId1"/>
-    <sheet name="Reconciliation Schedule" sheetId="2" r:id="rId2"/>
+    <sheet name="Reconciliation Statement" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>STATEMENT OF CASH FLOW (in millions of $)</t>
   </si>
@@ -118,6 +117,39 @@
   </si>
   <si>
     <t xml:space="preserve">           Total Cash disimbursement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATEMENT OF RECONCILIATION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Income </t>
+  </si>
+  <si>
+    <t>Depreciation &amp; amortization</t>
+  </si>
+  <si>
+    <t>to the net cash flow from operation:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Increase in Accounts Recievable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Increase in Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Increase in Accounts Payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Increase in Accrued Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Increase in Income Taxes Accrued</t>
+  </si>
+  <si>
+    <t>Adjustments to reconcile net income</t>
+  </si>
+  <si>
+    <t>Net cash flow from operation</t>
   </si>
 </sst>
 </file>
@@ -512,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59459543-48CD-461C-9EC4-AD6EE0DD6E09}">
-  <dimension ref="I5:M38"/>
+  <dimension ref="I5:W38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,31 +556,47 @@
     <col min="11" max="11" width="2.6640625" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" customWidth="1"/>
     <col min="13" max="13" width="11.77734375" customWidth="1"/>
+    <col min="19" max="19" width="27.6640625" customWidth="1"/>
+    <col min="21" max="21" width="3.6640625" customWidth="1"/>
+    <col min="22" max="22" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="9:23" x14ac:dyDescent="0.3">
       <c r="K5" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="U5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="9:23" x14ac:dyDescent="0.3">
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I7" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S7" t="s">
+        <v>5</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="9:23" x14ac:dyDescent="0.3">
       <c r="L8" s="7" t="s">
         <v>2</v>
       </c>
       <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="V8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I9" s="6" t="s">
         <v>1</v>
       </c>
@@ -558,13 +606,28 @@
       <c r="M9" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I11" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I12" t="s">
         <v>8</v>
       </c>
@@ -572,29 +635,41 @@
       <c r="M12" s="4">
         <v>1390</v>
       </c>
-    </row>
-    <row r="13" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S12" t="s">
+        <v>29</v>
+      </c>
+      <c r="W12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I14" t="s">
         <v>10</v>
       </c>
       <c r="L14">
         <v>-815</v>
       </c>
-    </row>
-    <row r="15" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I15" t="s">
         <v>11</v>
       </c>
       <c r="L15">
         <v>-200</v>
       </c>
-    </row>
-    <row r="16" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
         <v>12</v>
       </c>
@@ -602,15 +677,21 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
         <v>13</v>
       </c>
       <c r="L17">
         <v>-100</v>
       </c>
-    </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S17" t="s">
+        <v>31</v>
+      </c>
+      <c r="W17">
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="18" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
         <v>26</v>
       </c>
@@ -618,16 +699,44 @@
         <f>SUM(L14:L17)</f>
         <v>-1128</v>
       </c>
-    </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S18" t="s">
+        <v>32</v>
+      </c>
+      <c r="W18">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="19" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S19" t="s">
+        <v>33</v>
+      </c>
+      <c r="W19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
         <v>14</v>
       </c>
       <c r="M20">
         <v>-35</v>
       </c>
-    </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="S20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="21" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S21" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I22" s="3" t="s">
         <v>15</v>
       </c>
@@ -636,12 +745,21 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="9:23" x14ac:dyDescent="0.3">
+      <c r="S23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W23" s="3">
+        <f>SUM(W11:W22)</f>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I24" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>17</v>
       </c>
@@ -649,7 +767,7 @@
         <v>-435</v>
       </c>
     </row>
-    <row r="26" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I26" t="s">
         <v>18</v>
       </c>
@@ -657,7 +775,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I28" s="3" t="s">
         <v>19</v>
       </c>
@@ -666,12 +784,12 @@
         <v>-310</v>
       </c>
     </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I30" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I31" t="s">
         <v>21</v>
       </c>
@@ -715,23 +833,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="V8:W8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7EB2149-AB48-4718-98B1-56933EB2EE89}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>